<commit_message>
Send error for IMU steering
</commit_message>
<xml_diff>
--- a/Support/PGN 5.1.xlsx
+++ b/Support/PGN 5.1.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24012"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="65" documentId="11_8BAB8071C68B353072354CC245F0B79A2C73F9FF" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8DBB1862-8BB3-4F76-8049-2510D0F23E27}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="PGN" sheetId="1" r:id="rId1"/>
     <sheet name="fixed IP list" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="101">
   <si>
     <t>Format: 0x80, 0x81, Src, PGN, Length, [Data Bytes], CRC</t>
   </si>
@@ -296,18 +295,9 @@
     <t>Seconds</t>
   </si>
   <si>
-    <t>LatLon</t>
-  </si>
-  <si>
     <t>D0</t>
   </si>
   <si>
-    <t>Latitude encoded 4 byte /90.0</t>
-  </si>
-  <si>
-    <t>Longitude encoded 4 byte /180.0</t>
-  </si>
-  <si>
     <t>IP Addresses when using fixed IPs</t>
   </si>
   <si>
@@ -336,13 +326,16 @@
   </si>
   <si>
     <t>Tablet Computer</t>
+  </si>
+  <si>
+    <t>Gyro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,7 +417,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -597,21 +590,10 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -758,31 +740,31 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -845,7 +827,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -897,7 +879,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1091,21 +1073,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="34" customWidth="1"/>
     <col min="2" max="4" width="5.140625" style="6" customWidth="1"/>
@@ -1116,16 +1098,16 @@
     <col min="19" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14.25" customHeight="1">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -1135,7 +1117,7 @@
       <c r="N1" s="44"/>
       <c r="O1" s="44"/>
     </row>
-    <row r="2" spans="1:18" s="9" customFormat="1" ht="14.25">
+    <row r="2" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1155,7 +1137,7 @@
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
     </row>
-    <row r="3" spans="1:18" s="18" customFormat="1">
+    <row r="3" spans="1:18" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
@@ -1209,7 +1191,7 @@
       </c>
       <c r="R3" s="17"/>
     </row>
-    <row r="4" spans="1:18" s="9" customFormat="1" ht="14.25">
+    <row r="4" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="19"/>
       <c r="B4" s="20"/>
       <c r="C4" s="21"/>
@@ -1229,7 +1211,7 @@
       <c r="Q4" s="28"/>
       <c r="R4" s="8"/>
     </row>
-    <row r="5" spans="1:18" ht="14.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>18</v>
       </c>
@@ -1246,17 +1228,17 @@
       <c r="E5" s="22">
         <v>8</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="56"/>
+      <c r="G5" s="52"/>
       <c r="H5" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="57" t="s">
+      <c r="I5" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="58"/>
+      <c r="J5" s="54"/>
       <c r="K5" s="44" t="s">
         <v>24</v>
       </c>
@@ -1272,7 +1254,7 @@
       <c r="O5" s="32"/>
       <c r="P5" s="33"/>
     </row>
-    <row r="6" spans="1:18" ht="14.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="D6" s="43"/>
@@ -1287,7 +1269,7 @@
       <c r="N6" s="44"/>
       <c r="O6" s="44"/>
     </row>
-    <row r="7" spans="1:18" ht="14.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="34" t="s">
         <v>28</v>
       </c>
@@ -1304,18 +1286,18 @@
       <c r="E7" s="22">
         <v>8</v>
       </c>
-      <c r="F7" s="53" t="s">
+      <c r="F7" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50" t="s">
+      <c r="G7" s="56"/>
+      <c r="H7" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50" t="s">
+      <c r="I7" s="56"/>
+      <c r="J7" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="50"/>
+      <c r="K7" s="56"/>
       <c r="L7" s="44" t="s">
         <v>34</v>
       </c>
@@ -1327,7 +1309,7 @@
       </c>
       <c r="O7" s="44"/>
     </row>
-    <row r="8" spans="1:18" ht="14.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B8" s="43"/>
       <c r="C8" s="43"/>
       <c r="D8" s="43"/>
@@ -1342,7 +1324,7 @@
       <c r="N8" s="44"/>
       <c r="O8" s="44"/>
     </row>
-    <row r="9" spans="1:18" ht="14.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="34" t="s">
         <v>36</v>
       </c>
@@ -1374,10 +1356,10 @@
       <c r="J9" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="50" t="s">
+      <c r="K9" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="50"/>
+      <c r="L9" s="56"/>
       <c r="M9" s="44" t="s">
         <v>44</v>
       </c>
@@ -1386,7 +1368,7 @@
       </c>
       <c r="O9" s="44"/>
     </row>
-    <row r="10" spans="1:18" ht="14.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B10" s="43"/>
       <c r="C10" s="43"/>
       <c r="D10" s="43"/>
@@ -1401,7 +1383,7 @@
       <c r="N10" s="44"/>
       <c r="O10" s="44"/>
     </row>
-    <row r="11" spans="1:18" ht="14.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="34" t="s">
         <v>45</v>
       </c>
@@ -1447,7 +1429,7 @@
       </c>
       <c r="O11" s="44"/>
     </row>
-    <row r="12" spans="1:18" ht="14.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B12" s="43"/>
       <c r="C12" s="43"/>
       <c r="D12" s="43"/>
@@ -1462,7 +1444,7 @@
       <c r="N12" s="44"/>
       <c r="O12" s="44"/>
     </row>
-    <row r="13" spans="1:18" s="40" customFormat="1" ht="14.25">
+    <row r="13" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="35"/>
       <c r="B13" s="36"/>
       <c r="C13" s="36"/>
@@ -1482,7 +1464,7 @@
       <c r="Q13" s="39"/>
       <c r="R13" s="39"/>
     </row>
-    <row r="14" spans="1:18" ht="14.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="34" t="s">
         <v>51</v>
       </c>
@@ -1528,7 +1510,7 @@
       </c>
       <c r="O14" s="44"/>
     </row>
-    <row r="15" spans="1:18" ht="14.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B15" s="43"/>
       <c r="C15" s="43"/>
       <c r="D15" s="43"/>
@@ -1543,7 +1525,7 @@
       <c r="N15" s="44"/>
       <c r="O15" s="44"/>
     </row>
-    <row r="16" spans="1:18" ht="14.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="34" t="s">
         <v>57</v>
       </c>
@@ -1587,7 +1569,7 @@
       </c>
       <c r="O16" s="44"/>
     </row>
-    <row r="17" spans="1:18" ht="14.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B17" s="43"/>
       <c r="C17" s="43"/>
       <c r="D17" s="43"/>
@@ -1602,13 +1584,13 @@
       <c r="N17" s="44"/>
       <c r="O17" s="44"/>
     </row>
-    <row r="18" spans="1:18" ht="14.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B18" s="43"/>
       <c r="C18" s="43" t="s">
         <v>62</v>
       </c>
       <c r="D18" s="43">
-        <f t="shared" ref="D18:D19" si="0">HEX2DEC(C18)</f>
+        <f t="shared" ref="D18" si="0">HEX2DEC(C18)</f>
         <v>237</v>
       </c>
       <c r="F18" s="44"/>
@@ -1622,7 +1604,7 @@
       <c r="N18" s="44"/>
       <c r="O18" s="44"/>
     </row>
-    <row r="19" spans="1:18" ht="14.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B19" s="43"/>
       <c r="C19" s="43"/>
       <c r="D19" s="43"/>
@@ -1637,7 +1619,7 @@
       <c r="N19" s="44"/>
       <c r="O19" s="44"/>
     </row>
-    <row r="20" spans="1:18" ht="14.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B20" s="43"/>
       <c r="C20" s="43"/>
       <c r="D20" s="43"/>
@@ -1652,7 +1634,7 @@
       <c r="N20" s="44"/>
       <c r="O20" s="44"/>
     </row>
-    <row r="21" spans="1:18" ht="14.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B21" s="43"/>
       <c r="C21" s="43"/>
       <c r="D21" s="43"/>
@@ -1667,7 +1649,7 @@
       <c r="N21" s="44"/>
       <c r="O21" s="44"/>
     </row>
-    <row r="22" spans="1:18" ht="14.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="34" t="s">
         <v>63</v>
       </c>
@@ -1709,7 +1691,7 @@
       </c>
       <c r="O22" s="3"/>
     </row>
-    <row r="23" spans="1:18" ht="14.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B23" s="43"/>
       <c r="C23" s="43"/>
       <c r="D23" s="43"/>
@@ -1724,7 +1706,7 @@
       <c r="N23" s="44"/>
       <c r="O23" s="44"/>
     </row>
-    <row r="24" spans="1:18" ht="14.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B24" s="43"/>
       <c r="C24" s="43"/>
       <c r="D24" s="43"/>
@@ -1739,7 +1721,7 @@
       <c r="N24" s="44"/>
       <c r="O24" s="44"/>
     </row>
-    <row r="25" spans="1:18" ht="14.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B25" s="43"/>
       <c r="C25" s="43"/>
       <c r="D25" s="43"/>
@@ -1754,7 +1736,7 @@
       <c r="N25" s="44"/>
       <c r="O25" s="44"/>
     </row>
-    <row r="26" spans="1:18" s="40" customFormat="1" ht="14.25">
+    <row r="26" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="35"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -1774,7 +1756,7 @@
       <c r="Q26" s="39"/>
       <c r="R26" s="39"/>
     </row>
-    <row r="27" spans="1:18" s="49" customFormat="1" ht="14.25">
+    <row r="27" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="45" t="s">
         <v>73</v>
       </c>
@@ -1804,7 +1786,7 @@
       <c r="Q27" s="48"/>
       <c r="R27" s="48"/>
     </row>
-    <row r="28" spans="1:18" s="49" customFormat="1" ht="14.25">
+    <row r="28" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="45"/>
       <c r="B28" s="46"/>
       <c r="C28" s="46"/>
@@ -1824,7 +1806,7 @@
       <c r="Q28" s="48"/>
       <c r="R28" s="48"/>
     </row>
-    <row r="29" spans="1:18" ht="14.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="34" t="s">
         <v>77</v>
       </c>
@@ -1857,7 +1839,7 @@
       <c r="N29" s="44"/>
       <c r="O29" s="44"/>
     </row>
-    <row r="30" spans="1:18" ht="14.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B30" s="43"/>
       <c r="C30" s="43"/>
       <c r="D30" s="43"/>
@@ -1872,7 +1854,7 @@
       <c r="N30" s="44"/>
       <c r="O30" s="44"/>
     </row>
-    <row r="31" spans="1:18" ht="14.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="34" t="s">
         <v>81</v>
       </c>
@@ -1886,27 +1868,33 @@
         <f>HEX2DEC(C31)</f>
         <v>211</v>
       </c>
-      <c r="E31" s="22">
-        <v>4</v>
-      </c>
-      <c r="F31" s="51" t="s">
+      <c r="E31" s="46">
+        <v>8</v>
+      </c>
+      <c r="F31" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52" t="s">
+      <c r="G31" s="57"/>
+      <c r="H31" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="I31" s="52"/>
-      <c r="J31" s="44" t="s">
+      <c r="I31" s="57"/>
+      <c r="J31" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="K31" s="56"/>
+      <c r="L31" s="44">
+        <v>0</v>
+      </c>
+      <c r="M31" s="44">
+        <v>0</v>
+      </c>
+      <c r="N31" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="K31" s="44"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="44"/>
-      <c r="N31" s="44"/>
       <c r="O31" s="44"/>
     </row>
-    <row r="32" spans="1:18" ht="14.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B32" s="43"/>
       <c r="C32" s="43"/>
       <c r="D32" s="43"/>
@@ -1921,7 +1909,7 @@
       <c r="N32" s="44"/>
       <c r="O32" s="44"/>
     </row>
-    <row r="33" spans="1:15" ht="14.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="34" t="s">
         <v>86</v>
       </c>
@@ -1951,7 +1939,7 @@
       <c r="N33" s="44"/>
       <c r="O33" s="44"/>
     </row>
-    <row r="34" spans="1:15" ht="14.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B34" s="43"/>
       <c r="C34" s="43"/>
       <c r="D34" s="43"/>
@@ -1966,7 +1954,7 @@
       <c r="N34" s="44"/>
       <c r="O34" s="44"/>
     </row>
-    <row r="35" spans="1:15" ht="14.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B35" s="43" t="s">
         <v>19</v>
       </c>
@@ -1975,18 +1963,18 @@
         <f>HEX2DEC(C35)</f>
         <v>0</v>
       </c>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="50"/>
-      <c r="L35" s="50"/>
-      <c r="M35" s="50"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="56"/>
+      <c r="L35" s="56"/>
+      <c r="M35" s="56"/>
       <c r="N35" s="44"/>
       <c r="O35" s="44"/>
     </row>
-    <row r="36" spans="1:15" ht="14.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B36" s="43"/>
       <c r="C36" s="43"/>
       <c r="D36" s="43"/>
@@ -2001,41 +1989,26 @@
       <c r="N36" s="44"/>
       <c r="O36" s="44"/>
     </row>
-    <row r="37" spans="1:15" ht="14.25">
-      <c r="A37" s="34" t="s">
-        <v>89</v>
-      </c>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B37" s="43" t="s">
         <v>19</v>
       </c>
       <c r="C37" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="D37" s="43">
-        <f>HEX2DEC(C37)</f>
-        <v>208</v>
-      </c>
-      <c r="E37" s="22">
-        <v>8</v>
-      </c>
-      <c r="F37" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="G37" s="50"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="K37" s="50"/>
-      <c r="L37" s="50"/>
-      <c r="M37" s="50"/>
-      <c r="N37" s="44" t="s">
-        <v>27</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="D37" s="43"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="56"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="56"/>
+      <c r="J37" s="56"/>
+      <c r="K37" s="56"/>
+      <c r="L37" s="56"/>
+      <c r="M37" s="56"/>
+      <c r="N37" s="44"/>
       <c r="O37" s="44"/>
     </row>
-    <row r="38" spans="1:15" ht="14.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B38" s="43"/>
       <c r="C38" s="43"/>
       <c r="D38" s="43"/>
@@ -2050,7 +2023,7 @@
       <c r="N38" s="44"/>
       <c r="O38" s="44"/>
     </row>
-    <row r="39" spans="1:15" ht="14.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B39" s="43"/>
       <c r="C39" s="43"/>
       <c r="D39" s="43"/>
@@ -2065,7 +2038,7 @@
       <c r="N39" s="44"/>
       <c r="O39" s="44"/>
     </row>
-    <row r="40" spans="1:15" ht="14.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B40" s="43"/>
       <c r="C40" s="43"/>
       <c r="D40" s="43"/>
@@ -2080,7 +2053,7 @@
       <c r="N40" s="44"/>
       <c r="O40" s="44"/>
     </row>
-    <row r="41" spans="1:15" ht="14.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B41" s="43"/>
       <c r="C41" s="43"/>
       <c r="D41" s="43"/>
@@ -2095,7 +2068,7 @@
       <c r="N41" s="44"/>
       <c r="O41" s="44"/>
     </row>
-    <row r="43" spans="1:15" ht="14.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B43" s="43"/>
       <c r="C43" s="43"/>
       <c r="D43" s="43"/>
@@ -2110,7 +2083,7 @@
       <c r="N43" s="44"/>
       <c r="O43" s="44"/>
     </row>
-    <row r="45" spans="1:15" ht="14.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B45" s="43"/>
       <c r="C45" s="43"/>
       <c r="D45" s="43"/>
@@ -2125,7 +2098,7 @@
       <c r="N45" s="44"/>
       <c r="O45" s="44"/>
     </row>
-    <row r="47" spans="1:15" ht="14.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B47" s="43"/>
       <c r="C47" s="43"/>
       <c r="D47" s="43"/>
@@ -2140,7 +2113,7 @@
       <c r="N47" s="44"/>
       <c r="O47" s="44"/>
     </row>
-    <row r="48" spans="1:15" ht="14.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B48" s="43"/>
       <c r="C48" s="43"/>
       <c r="D48" s="43"/>
@@ -2155,7 +2128,7 @@
       <c r="N48" s="44"/>
       <c r="O48" s="44"/>
     </row>
-    <row r="49" spans="2:15" ht="14.25">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B49" s="43"/>
       <c r="C49" s="43"/>
       <c r="D49" s="43"/>
@@ -2170,7 +2143,7 @@
       <c r="N49" s="44"/>
       <c r="O49" s="44"/>
     </row>
-    <row r="50" spans="2:15" ht="14.25">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B50" s="43"/>
       <c r="C50" s="43"/>
       <c r="D50" s="43"/>
@@ -2185,7 +2158,7 @@
       <c r="N50" s="44"/>
       <c r="O50" s="44"/>
     </row>
-    <row r="51" spans="2:15" ht="14.25">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B51" s="43"/>
       <c r="C51" s="43"/>
       <c r="D51" s="43"/>
@@ -2200,7 +2173,7 @@
       <c r="N51" s="44"/>
       <c r="O51" s="44"/>
     </row>
-    <row r="53" spans="2:15" ht="14.25">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B53" s="43"/>
       <c r="C53" s="43"/>
       <c r="D53" s="43"/>
@@ -2215,7 +2188,7 @@
       <c r="N53" s="44"/>
       <c r="O53" s="44"/>
     </row>
-    <row r="55" spans="2:15" ht="14.25">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B55" s="43"/>
       <c r="C55" s="43"/>
       <c r="D55" s="43"/>
@@ -2230,7 +2203,7 @@
       <c r="N55" s="44"/>
       <c r="O55" s="44"/>
     </row>
-    <row r="56" spans="2:15" ht="14.25">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B56" s="43"/>
       <c r="C56" s="43"/>
       <c r="D56" s="43"/>
@@ -2245,7 +2218,7 @@
       <c r="N56" s="44"/>
       <c r="O56" s="44"/>
     </row>
-    <row r="57" spans="2:15" ht="14.25">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B57" s="43"/>
       <c r="C57" s="43"/>
       <c r="D57" s="43"/>
@@ -2260,7 +2233,7 @@
       <c r="N57" s="44"/>
       <c r="O57" s="44"/>
     </row>
-    <row r="58" spans="2:15" ht="14.25">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B58" s="43"/>
       <c r="C58" s="43"/>
       <c r="D58" s="43"/>
@@ -2275,7 +2248,7 @@
       <c r="N58" s="44"/>
       <c r="O58" s="44"/>
     </row>
-    <row r="59" spans="2:15" ht="14.25">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B59" s="43"/>
       <c r="C59" s="43"/>
       <c r="D59" s="43"/>
@@ -2290,7 +2263,7 @@
       <c r="N59" s="44"/>
       <c r="O59" s="44"/>
     </row>
-    <row r="60" spans="2:15" ht="14.25">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B60" s="43"/>
       <c r="C60" s="43"/>
       <c r="D60" s="43"/>
@@ -2305,7 +2278,7 @@
       <c r="N60" s="44"/>
       <c r="O60" s="44"/>
     </row>
-    <row r="61" spans="2:15" ht="14.25">
+    <row r="61" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B61" s="43"/>
       <c r="C61" s="43"/>
       <c r="D61" s="43"/>
@@ -2320,7 +2293,7 @@
       <c r="N61" s="44"/>
       <c r="O61" s="44"/>
     </row>
-    <row r="62" spans="2:15" ht="14.25">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B62" s="43"/>
       <c r="C62" s="43"/>
       <c r="D62" s="43"/>
@@ -2335,7 +2308,7 @@
       <c r="N62" s="44"/>
       <c r="O62" s="44"/>
     </row>
-    <row r="63" spans="2:15" ht="14.25">
+    <row r="63" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B63" s="43"/>
       <c r="C63" s="43"/>
       <c r="D63" s="43"/>
@@ -2350,7 +2323,7 @@
       <c r="N63" s="44"/>
       <c r="O63" s="44"/>
     </row>
-    <row r="64" spans="2:15" ht="14.25">
+    <row r="64" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B64" s="43"/>
       <c r="C64" s="43"/>
       <c r="D64" s="43"/>
@@ -2366,93 +2339,94 @@
       <c r="O64" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="F35:M35"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="J31:K31"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="J7:K7"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="F35:M35"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="J37:M37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B28BA9E-E025-4F56-A049-31FC3C6329F7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>75</v>
       </c>
@@ -2460,10 +2434,10 @@
         <v>81</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>76</v>
       </c>
@@ -2471,69 +2445,69 @@
         <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>80</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>100</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2542,6 +2516,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100168D69F7049F5C4D941A1ED43A3EBF4E" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="6358b93c66be89da512ed1b0037fb663">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ac7999f6-dd20-429f-9c50-d27a0c8de317" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7603896104695ce44c6e748634a25e45" ns2:_="">
     <xsd:import namespace="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
@@ -2705,15 +2688,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2721,13 +2695,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F34BA2AD-7737-4D5E-9A5C-0001377CDA31}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F34BA2AD-7737-4D5E-9A5C-0001377CDA31}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
UDP INO reset pgn fix
</commit_message>
<xml_diff>
--- a/Support/PGN 5.1.xlsx
+++ b/Support/PGN 5.1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="104">
   <si>
     <t>Format: 0x80, 0x81, Src, PGN, Length, [Data Bytes], CRC</t>
   </si>
@@ -329,6 +329,15 @@
   </si>
   <si>
     <t>Gyro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7F </t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>Hello AOG</t>
   </si>
 </sst>
 </file>
@@ -740,6 +749,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -753,18 +774,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1073,7 +1082,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1083,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1099,15 +1108,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -1228,17 +1237,17 @@
       <c r="E5" s="22">
         <v>8</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="52"/>
+      <c r="G5" s="56"/>
       <c r="H5" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="53" t="s">
+      <c r="I5" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="54"/>
+      <c r="J5" s="58"/>
       <c r="K5" s="44" t="s">
         <v>24</v>
       </c>
@@ -1286,18 +1295,18 @@
       <c r="E7" s="22">
         <v>8</v>
       </c>
-      <c r="F7" s="55" t="s">
+      <c r="F7" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56" t="s">
+      <c r="G7" s="50"/>
+      <c r="H7" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56" t="s">
+      <c r="I7" s="50"/>
+      <c r="J7" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="56"/>
+      <c r="K7" s="50"/>
       <c r="L7" s="44" t="s">
         <v>34</v>
       </c>
@@ -1356,10 +1365,10 @@
       <c r="J9" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="56" t="s">
+      <c r="K9" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="56"/>
+      <c r="L9" s="50"/>
       <c r="M9" s="44" t="s">
         <v>44</v>
       </c>
@@ -1871,18 +1880,18 @@
       <c r="E31" s="46">
         <v>8</v>
       </c>
-      <c r="F31" s="58" t="s">
+      <c r="F31" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="G31" s="57"/>
-      <c r="H31" s="57" t="s">
+      <c r="G31" s="52"/>
+      <c r="H31" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="I31" s="57"/>
-      <c r="J31" s="56" t="s">
+      <c r="I31" s="52"/>
+      <c r="J31" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="K31" s="56"/>
+      <c r="K31" s="50"/>
       <c r="L31" s="44">
         <v>0</v>
       </c>
@@ -1963,14 +1972,14 @@
         <f>HEX2DEC(C35)</f>
         <v>0</v>
       </c>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="56"/>
-      <c r="K35" s="56"/>
-      <c r="L35" s="56"/>
-      <c r="M35" s="56"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
+      <c r="K35" s="50"/>
+      <c r="L35" s="50"/>
+      <c r="M35" s="50"/>
       <c r="N35" s="44"/>
       <c r="O35" s="44"/>
     </row>
@@ -1997,14 +2006,14 @@
         <v>89</v>
       </c>
       <c r="D37" s="43"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="56"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="56"/>
-      <c r="M37" s="56"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="50"/>
+      <c r="L37" s="50"/>
+      <c r="M37" s="50"/>
       <c r="N37" s="44"/>
       <c r="O37" s="44"/>
     </row>
@@ -2024,11 +2033,22 @@
       <c r="O38" s="44"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
+      <c r="A39" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="43" t="s">
+        <v>102</v>
+      </c>
       <c r="D39" s="43"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="44"/>
+      <c r="F39" s="44">
+        <v>1</v>
+      </c>
+      <c r="G39" s="44" t="s">
+        <v>27</v>
+      </c>
       <c r="H39" s="44"/>
       <c r="I39" s="44"/>
       <c r="J39" s="44"/>
@@ -2340,6 +2360,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="H31:I31"/>
@@ -2347,12 +2373,6 @@
     <mergeCell ref="F37:I37"/>
     <mergeCell ref="J37:M37"/>
     <mergeCell ref="J31:K31"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2516,15 +2536,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100168D69F7049F5C4D941A1ED43A3EBF4E" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="6358b93c66be89da512ed1b0037fb663">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ac7999f6-dd20-429f-9c50-d27a0c8de317" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7603896104695ce44c6e748634a25e45" ns2:_="">
     <xsd:import namespace="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
@@ -2688,6 +2699,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2695,14 +2715,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F34BA2AD-7737-4D5E-9A5C-0001377CDA31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2720,6 +2732,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Relay Config with new Machine Module 5_4
</commit_message>
<xml_diff>
--- a/Support/PGN 5.1.xlsx
+++ b/Support/PGN 5.1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="105">
   <si>
     <t>Format: 0x80, 0x81, Src, PGN, Length, [Data Bytes], CRC</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>Hello AOG</t>
+  </si>
+  <si>
+    <t>relayConfig</t>
   </si>
 </sst>
 </file>
@@ -749,6 +752,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -756,24 +777,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1082,7 +1085,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1090,10 +1093,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R64"/>
+  <dimension ref="A1:Z64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1108,15 +1111,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -1237,17 +1240,17 @@
       <c r="E5" s="22">
         <v>8</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="56"/>
+      <c r="G5" s="52"/>
       <c r="H5" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="57" t="s">
+      <c r="I5" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="58"/>
+      <c r="J5" s="54"/>
       <c r="K5" s="44" t="s">
         <v>24</v>
       </c>
@@ -1295,18 +1298,18 @@
       <c r="E7" s="22">
         <v>8</v>
       </c>
-      <c r="F7" s="53" t="s">
+      <c r="F7" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50" t="s">
+      <c r="G7" s="56"/>
+      <c r="H7" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50" t="s">
+      <c r="I7" s="56"/>
+      <c r="J7" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="50"/>
+      <c r="K7" s="56"/>
       <c r="L7" s="44" t="s">
         <v>34</v>
       </c>
@@ -1365,10 +1368,10 @@
       <c r="J9" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="50" t="s">
+      <c r="K9" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="50"/>
+      <c r="L9" s="56"/>
       <c r="M9" s="44" t="s">
         <v>44</v>
       </c>
@@ -1578,7 +1581,7 @@
       </c>
       <c r="O16" s="44"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B17" s="43"/>
       <c r="C17" s="43"/>
       <c r="D17" s="43"/>
@@ -1593,7 +1596,10 @@
       <c r="N17" s="44"/>
       <c r="O17" s="44"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A18" s="34" t="s">
+        <v>104</v>
+      </c>
       <c r="B18" s="43"/>
       <c r="C18" s="43" t="s">
         <v>62</v>
@@ -1602,18 +1608,74 @@
         <f t="shared" ref="D18" si="0">HEX2DEC(C18)</f>
         <v>237</v>
       </c>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="44"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="44"/>
-      <c r="N18" s="44"/>
-      <c r="O18" s="44"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E18" s="22">
+        <v>20</v>
+      </c>
+      <c r="F18" s="44">
+        <v>1</v>
+      </c>
+      <c r="G18" s="44">
+        <v>2</v>
+      </c>
+      <c r="H18" s="44">
+        <v>3</v>
+      </c>
+      <c r="I18" s="44">
+        <v>4</v>
+      </c>
+      <c r="J18" s="44">
+        <v>5</v>
+      </c>
+      <c r="K18" s="44">
+        <v>6</v>
+      </c>
+      <c r="L18" s="44">
+        <v>7</v>
+      </c>
+      <c r="M18" s="44">
+        <v>8</v>
+      </c>
+      <c r="N18" s="44">
+        <v>9</v>
+      </c>
+      <c r="O18" s="44">
+        <v>10</v>
+      </c>
+      <c r="P18" s="2">
+        <v>11</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>12</v>
+      </c>
+      <c r="R18" s="2">
+        <v>13</v>
+      </c>
+      <c r="S18" s="3">
+        <v>14</v>
+      </c>
+      <c r="T18" s="3">
+        <v>15</v>
+      </c>
+      <c r="U18" s="3">
+        <v>16</v>
+      </c>
+      <c r="V18" s="3">
+        <v>17</v>
+      </c>
+      <c r="W18" s="3">
+        <v>18</v>
+      </c>
+      <c r="X18" s="3">
+        <v>19</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>20</v>
+      </c>
+      <c r="Z18" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B19" s="43"/>
       <c r="C19" s="43"/>
       <c r="D19" s="43"/>
@@ -1628,7 +1690,7 @@
       <c r="N19" s="44"/>
       <c r="O19" s="44"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B20" s="43"/>
       <c r="C20" s="43"/>
       <c r="D20" s="43"/>
@@ -1643,7 +1705,7 @@
       <c r="N20" s="44"/>
       <c r="O20" s="44"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B21" s="43"/>
       <c r="C21" s="43"/>
       <c r="D21" s="43"/>
@@ -1658,7 +1720,7 @@
       <c r="N21" s="44"/>
       <c r="O21" s="44"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="34" t="s">
         <v>63</v>
       </c>
@@ -1700,7 +1762,7 @@
       </c>
       <c r="O22" s="3"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B23" s="43"/>
       <c r="C23" s="43"/>
       <c r="D23" s="43"/>
@@ -1715,7 +1777,7 @@
       <c r="N23" s="44"/>
       <c r="O23" s="44"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B24" s="43"/>
       <c r="C24" s="43"/>
       <c r="D24" s="43"/>
@@ -1730,7 +1792,7 @@
       <c r="N24" s="44"/>
       <c r="O24" s="44"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B25" s="43"/>
       <c r="C25" s="43"/>
       <c r="D25" s="43"/>
@@ -1745,7 +1807,7 @@
       <c r="N25" s="44"/>
       <c r="O25" s="44"/>
     </row>
-    <row r="26" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="35"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -1765,7 +1827,7 @@
       <c r="Q26" s="39"/>
       <c r="R26" s="39"/>
     </row>
-    <row r="27" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="45" t="s">
         <v>73</v>
       </c>
@@ -1795,7 +1857,7 @@
       <c r="Q27" s="48"/>
       <c r="R27" s="48"/>
     </row>
-    <row r="28" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="45"/>
       <c r="B28" s="46"/>
       <c r="C28" s="46"/>
@@ -1815,7 +1877,7 @@
       <c r="Q28" s="48"/>
       <c r="R28" s="48"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="34" t="s">
         <v>77</v>
       </c>
@@ -1848,7 +1910,7 @@
       <c r="N29" s="44"/>
       <c r="O29" s="44"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B30" s="43"/>
       <c r="C30" s="43"/>
       <c r="D30" s="43"/>
@@ -1863,7 +1925,7 @@
       <c r="N30" s="44"/>
       <c r="O30" s="44"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" s="34" t="s">
         <v>81</v>
       </c>
@@ -1880,18 +1942,18 @@
       <c r="E31" s="46">
         <v>8</v>
       </c>
-      <c r="F31" s="51" t="s">
+      <c r="F31" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52" t="s">
+      <c r="G31" s="58"/>
+      <c r="H31" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="I31" s="52"/>
-      <c r="J31" s="50" t="s">
+      <c r="I31" s="58"/>
+      <c r="J31" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="K31" s="50"/>
+      <c r="K31" s="56"/>
       <c r="L31" s="44">
         <v>0</v>
       </c>
@@ -1903,7 +1965,7 @@
       </c>
       <c r="O31" s="44"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B32" s="43"/>
       <c r="C32" s="43"/>
       <c r="D32" s="43"/>
@@ -1972,14 +2034,14 @@
         <f>HEX2DEC(C35)</f>
         <v>0</v>
       </c>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="50"/>
-      <c r="L35" s="50"/>
-      <c r="M35" s="50"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="56"/>
+      <c r="L35" s="56"/>
+      <c r="M35" s="56"/>
       <c r="N35" s="44"/>
       <c r="O35" s="44"/>
     </row>
@@ -2006,14 +2068,14 @@
         <v>89</v>
       </c>
       <c r="D37" s="43"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="50"/>
-      <c r="K37" s="50"/>
-      <c r="L37" s="50"/>
-      <c r="M37" s="50"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="56"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="56"/>
+      <c r="J37" s="56"/>
+      <c r="K37" s="56"/>
+      <c r="L37" s="56"/>
+      <c r="M37" s="56"/>
       <c r="N37" s="44"/>
       <c r="O37" s="44"/>
     </row>
@@ -2360,12 +2422,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="H31:I31"/>
@@ -2373,6 +2429,12 @@
     <mergeCell ref="F37:I37"/>
     <mergeCell ref="J37:M37"/>
     <mergeCell ref="J31:K31"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2536,6 +2598,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100168D69F7049F5C4D941A1ED43A3EBF4E" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="6358b93c66be89da512ed1b0037fb663">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ac7999f6-dd20-429f-9c50-d27a0c8de317" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7603896104695ce44c6e748634a25e45" ns2:_="">
     <xsd:import namespace="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
@@ -2699,15 +2770,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2715,6 +2777,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F34BA2AD-7737-4D5E-9A5C-0001377CDA31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2732,14 +2802,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
MCP machine module, 24 pins
</commit_message>
<xml_diff>
--- a/Support/PGN 5.1.xlsx
+++ b/Support/PGN 5.1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="106">
   <si>
     <t>Format: 0x80, 0x81, Src, PGN, Length, [Data Bytes], CRC</t>
   </si>
@@ -190,9 +190,6 @@
     <t>uturn</t>
   </si>
   <si>
-    <t>tree</t>
-  </si>
-  <si>
     <t>hydLift</t>
   </si>
   <si>
@@ -341,6 +338,12 @@
   </si>
   <si>
     <t>relayConfig</t>
+  </si>
+  <si>
+    <t>speed*10</t>
+  </si>
+  <si>
+    <t>Geo Stop</t>
   </si>
 </sst>
 </file>
@@ -752,6 +755,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -765,18 +780,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1085,7 +1088,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1093,10 +1096,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z64"/>
+  <dimension ref="A1:AD64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1111,15 +1114,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -1240,17 +1243,17 @@
       <c r="E5" s="22">
         <v>8</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="52"/>
+      <c r="G5" s="56"/>
       <c r="H5" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="53" t="s">
+      <c r="I5" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="54"/>
+      <c r="J5" s="58"/>
       <c r="K5" s="44" t="s">
         <v>24</v>
       </c>
@@ -1298,18 +1301,18 @@
       <c r="E7" s="22">
         <v>8</v>
       </c>
-      <c r="F7" s="55" t="s">
+      <c r="F7" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56" t="s">
+      <c r="G7" s="50"/>
+      <c r="H7" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56" t="s">
+      <c r="I7" s="50"/>
+      <c r="J7" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="56"/>
+      <c r="K7" s="50"/>
       <c r="L7" s="44" t="s">
         <v>34</v>
       </c>
@@ -1368,10 +1371,10 @@
       <c r="J9" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="56" t="s">
+      <c r="K9" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="56"/>
+      <c r="L9" s="50"/>
       <c r="M9" s="44" t="s">
         <v>44</v>
       </c>
@@ -1497,16 +1500,16 @@
         <v>53</v>
       </c>
       <c r="G14" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="44" t="s">
+      <c r="I14" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="I14" s="32" t="s">
-        <v>56</v>
-      </c>
       <c r="J14" s="44" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="K14" s="44" t="s">
         <v>24</v>
@@ -1539,11 +1542,11 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="43"/>
       <c r="C16" s="43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" s="43">
         <f>HEX2DEC(C16)</f>
@@ -1553,13 +1556,13 @@
         <v>8</v>
       </c>
       <c r="F16" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="44" t="s">
+      <c r="H16" s="44" t="s">
         <v>60</v>
-      </c>
-      <c r="H16" s="44" t="s">
-        <v>61</v>
       </c>
       <c r="I16" s="44" t="s">
         <v>47</v>
@@ -1581,7 +1584,7 @@
       </c>
       <c r="O16" s="44"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B17" s="43"/>
       <c r="C17" s="43"/>
       <c r="D17" s="43"/>
@@ -1596,13 +1599,13 @@
       <c r="N17" s="44"/>
       <c r="O17" s="44"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B18" s="43"/>
       <c r="C18" s="43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D18" s="43">
         <f t="shared" ref="D18" si="0">HEX2DEC(C18)</f>
@@ -1671,11 +1674,23 @@
       <c r="Y18" s="3">
         <v>20</v>
       </c>
-      <c r="Z18" s="3" t="s">
+      <c r="Z18" s="3">
+        <v>21</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>22</v>
+      </c>
+      <c r="AB18" s="3">
+        <v>23</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>24</v>
+      </c>
+      <c r="AD18" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B19" s="43"/>
       <c r="C19" s="43"/>
       <c r="D19" s="43"/>
@@ -1690,7 +1705,7 @@
       <c r="N19" s="44"/>
       <c r="O19" s="44"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B20" s="43"/>
       <c r="C20" s="43"/>
       <c r="D20" s="43"/>
@@ -1705,7 +1720,7 @@
       <c r="N20" s="44"/>
       <c r="O20" s="44"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B21" s="43"/>
       <c r="C21" s="43"/>
       <c r="D21" s="43"/>
@@ -1720,49 +1735,49 @@
       <c r="N21" s="44"/>
       <c r="O21" s="44"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="43" t="s">
+      <c r="C22" s="43" t="s">
         <v>64</v>
-      </c>
-      <c r="C22" s="43" t="s">
-        <v>65</v>
       </c>
       <c r="D22" s="43">
         <v>234</v>
       </c>
       <c r="F22" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="G22" s="44" t="s">
+      <c r="H22" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="I22" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="H22" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="I22" s="44" t="s">
+      <c r="J22" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="J22" s="44" t="s">
+      <c r="K22" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="K22" s="44" t="s">
+      <c r="L22" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="L22" s="44" t="s">
+      <c r="M22" s="44" t="s">
         <v>71</v>
-      </c>
-      <c r="M22" s="44" t="s">
-        <v>72</v>
       </c>
       <c r="N22" s="44" t="s">
         <v>27</v>
       </c>
       <c r="O22" s="3"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B23" s="43"/>
       <c r="C23" s="43"/>
       <c r="D23" s="43"/>
@@ -1777,7 +1792,7 @@
       <c r="N23" s="44"/>
       <c r="O23" s="44"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B24" s="43"/>
       <c r="C24" s="43"/>
       <c r="D24" s="43"/>
@@ -1792,7 +1807,7 @@
       <c r="N24" s="44"/>
       <c r="O24" s="44"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B25" s="43"/>
       <c r="C25" s="43"/>
       <c r="D25" s="43"/>
@@ -1807,7 +1822,7 @@
       <c r="N25" s="44"/>
       <c r="O25" s="44"/>
     </row>
-    <row r="26" spans="1:26" s="40" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="35"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -1827,21 +1842,21 @@
       <c r="Q26" s="39"/>
       <c r="R26" s="39"/>
     </row>
-    <row r="27" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="46" t="s">
+      <c r="C27" s="46" t="s">
         <v>74</v>
-      </c>
-      <c r="C27" s="46" t="s">
-        <v>75</v>
       </c>
       <c r="D27" s="46">
         <v>214</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F27" s="47"/>
       <c r="G27" s="47"/>
@@ -1857,7 +1872,7 @@
       <c r="Q27" s="48"/>
       <c r="R27" s="48"/>
     </row>
-    <row r="28" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="45"/>
       <c r="B28" s="46"/>
       <c r="C28" s="46"/>
@@ -1877,15 +1892,15 @@
       <c r="Q28" s="48"/>
       <c r="R28" s="48"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="43" t="s">
         <v>77</v>
-      </c>
-      <c r="B29" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="43" t="s">
-        <v>78</v>
       </c>
       <c r="D29" s="43">
         <v>212</v>
@@ -1894,10 +1909,10 @@
         <v>2</v>
       </c>
       <c r="F29" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" s="44" t="s">
         <v>79</v>
-      </c>
-      <c r="G29" s="44" t="s">
-        <v>80</v>
       </c>
       <c r="H29" s="44" t="s">
         <v>27</v>
@@ -1910,7 +1925,7 @@
       <c r="N29" s="44"/>
       <c r="O29" s="44"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B30" s="43"/>
       <c r="C30" s="43"/>
       <c r="D30" s="43"/>
@@ -1925,15 +1940,15 @@
       <c r="N30" s="44"/>
       <c r="O30" s="44"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="43" t="s">
+      <c r="C31" s="43" t="s">
         <v>82</v>
-      </c>
-      <c r="C31" s="43" t="s">
-        <v>83</v>
       </c>
       <c r="D31" s="43">
         <f>HEX2DEC(C31)</f>
@@ -1942,18 +1957,18 @@
       <c r="E31" s="46">
         <v>8</v>
       </c>
-      <c r="F31" s="57" t="s">
+      <c r="F31" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58" t="s">
-        <v>85</v>
-      </c>
-      <c r="I31" s="58"/>
-      <c r="J31" s="56" t="s">
-        <v>100</v>
-      </c>
-      <c r="K31" s="56"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="50" t="s">
+        <v>99</v>
+      </c>
+      <c r="K31" s="50"/>
       <c r="L31" s="44">
         <v>0</v>
       </c>
@@ -1965,7 +1980,7 @@
       </c>
       <c r="O31" s="44"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B32" s="43"/>
       <c r="C32" s="43"/>
       <c r="D32" s="43"/>
@@ -1982,23 +1997,23 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B33" s="43" t="s">
         <v>19</v>
       </c>
       <c r="C33" s="43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D33" s="43">
         <f>HEX2DEC(C33)</f>
         <v>210</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F33" s="44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="44"/>
       <c r="H33" s="44"/>
@@ -2034,14 +2049,14 @@
         <f>HEX2DEC(C35)</f>
         <v>0</v>
       </c>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="56"/>
-      <c r="K35" s="56"/>
-      <c r="L35" s="56"/>
-      <c r="M35" s="56"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
+      <c r="K35" s="50"/>
+      <c r="L35" s="50"/>
+      <c r="M35" s="50"/>
       <c r="N35" s="44"/>
       <c r="O35" s="44"/>
     </row>
@@ -2065,17 +2080,17 @@
         <v>19</v>
       </c>
       <c r="C37" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D37" s="43"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="56"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="56"/>
-      <c r="M37" s="56"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="50"/>
+      <c r="L37" s="50"/>
+      <c r="M37" s="50"/>
       <c r="N37" s="44"/>
       <c r="O37" s="44"/>
     </row>
@@ -2096,13 +2111,13 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B39" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="43" t="s">
         <v>101</v>
-      </c>
-      <c r="C39" s="43" t="s">
-        <v>102</v>
       </c>
       <c r="D39" s="43"/>
       <c r="F39" s="44">
@@ -2422,6 +2437,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="H31:I31"/>
@@ -2429,12 +2450,6 @@
     <mergeCell ref="F37:I37"/>
     <mergeCell ref="J37:M37"/>
     <mergeCell ref="J31:K31"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2455,17 +2470,17 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2473,7 +2488,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2481,10 +2496,10 @@
         <v>71</v>
       </c>
       <c r="B7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" t="s">
         <v>94</v>
-      </c>
-      <c r="C7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2492,10 +2507,10 @@
         <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2513,10 +2528,10 @@
         <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2524,10 +2539,10 @@
         <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2535,10 +2550,10 @@
         <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2546,10 +2561,10 @@
         <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2557,10 +2572,10 @@
         <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2568,10 +2583,10 @@
         <v>80</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2589,7 +2604,7 @@
         <v>100</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2598,15 +2613,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100168D69F7049F5C4D941A1ED43A3EBF4E" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="6358b93c66be89da512ed1b0037fb663">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ac7999f6-dd20-429f-9c50-d27a0c8de317" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7603896104695ce44c6e748634a25e45" ns2:_="">
     <xsd:import namespace="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
@@ -2770,6 +2776,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2777,14 +2792,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F34BA2AD-7737-4D5E-9A5C-0001377CDA31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2802,6 +2809,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
User fields for Machine, Add yaw to display
</commit_message>
<xml_diff>
--- a/Support/PGN 5.1.xlsx
+++ b/Support/PGN 5.1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="110">
   <si>
     <t>Format: 0x80, 0x81, Src, PGN, Length, [Data Bytes], CRC</t>
   </si>
@@ -344,6 +344,18 @@
   </si>
   <si>
     <t>Geo Stop</t>
+  </si>
+  <si>
+    <t>User1</t>
+  </si>
+  <si>
+    <t>User2</t>
+  </si>
+  <si>
+    <t>User3</t>
+  </si>
+  <si>
+    <t>User4</t>
   </si>
 </sst>
 </file>
@@ -755,6 +767,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -762,24 +792,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1088,7 +1100,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1099,7 +1111,7 @@
   <dimension ref="A1:AD64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1114,15 +1126,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -1243,17 +1255,17 @@
       <c r="E5" s="22">
         <v>8</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="56"/>
+      <c r="G5" s="52"/>
       <c r="H5" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="57" t="s">
+      <c r="I5" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="58"/>
+      <c r="J5" s="54"/>
       <c r="K5" s="44" t="s">
         <v>24</v>
       </c>
@@ -1301,18 +1313,18 @@
       <c r="E7" s="22">
         <v>8</v>
       </c>
-      <c r="F7" s="53" t="s">
+      <c r="F7" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50" t="s">
+      <c r="G7" s="56"/>
+      <c r="H7" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50" t="s">
+      <c r="I7" s="56"/>
+      <c r="J7" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="50"/>
+      <c r="K7" s="56"/>
       <c r="L7" s="44" t="s">
         <v>34</v>
       </c>
@@ -1371,10 +1383,10 @@
       <c r="J9" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="50" t="s">
+      <c r="K9" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="50"/>
+      <c r="L9" s="56"/>
       <c r="M9" s="44" t="s">
         <v>44</v>
       </c>
@@ -1568,16 +1580,16 @@
         <v>47</v>
       </c>
       <c r="J16" s="44" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="K16" s="44" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="L16" s="44" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="M16" s="44" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="N16" s="44" t="s">
         <v>27</v>
@@ -1957,18 +1969,18 @@
       <c r="E31" s="46">
         <v>8</v>
       </c>
-      <c r="F31" s="51" t="s">
+      <c r="F31" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52" t="s">
+      <c r="G31" s="58"/>
+      <c r="H31" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="I31" s="52"/>
-      <c r="J31" s="50" t="s">
+      <c r="I31" s="58"/>
+      <c r="J31" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="K31" s="50"/>
+      <c r="K31" s="56"/>
       <c r="L31" s="44">
         <v>0</v>
       </c>
@@ -2049,14 +2061,14 @@
         <f>HEX2DEC(C35)</f>
         <v>0</v>
       </c>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="50"/>
-      <c r="L35" s="50"/>
-      <c r="M35" s="50"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="56"/>
+      <c r="L35" s="56"/>
+      <c r="M35" s="56"/>
       <c r="N35" s="44"/>
       <c r="O35" s="44"/>
     </row>
@@ -2083,14 +2095,14 @@
         <v>88</v>
       </c>
       <c r="D37" s="43"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="50"/>
-      <c r="K37" s="50"/>
-      <c r="L37" s="50"/>
-      <c r="M37" s="50"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="56"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="56"/>
+      <c r="J37" s="56"/>
+      <c r="K37" s="56"/>
+      <c r="L37" s="56"/>
+      <c r="M37" s="56"/>
       <c r="N37" s="44"/>
       <c r="O37" s="44"/>
     </row>
@@ -2437,12 +2449,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="H31:I31"/>
@@ -2450,6 +2456,12 @@
     <mergeCell ref="F37:I37"/>
     <mergeCell ref="J37:M37"/>
     <mergeCell ref="J31:K31"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2613,6 +2625,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100168D69F7049F5C4D941A1ED43A3EBF4E" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="6358b93c66be89da512ed1b0037fb663">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ac7999f6-dd20-429f-9c50-d27a0c8de317" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7603896104695ce44c6e748634a25e45" ns2:_="">
     <xsd:import namespace="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
@@ -2776,15 +2797,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2792,6 +2804,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F34BA2AD-7737-4D5E-9A5C-0001377CDA31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2809,14 +2829,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Revert "Update PGN 5.1.xlsx"
This reverts commit 07949bda8683da2a9f9d5003cdccb35f272e382c.
</commit_message>
<xml_diff>
--- a/Support/PGN 5.1.xlsx
+++ b/Support/PGN 5.1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="110">
   <si>
     <t>Format: 0x80, 0x81, Src, PGN, Length, [Data Bytes], CRC</t>
   </si>
@@ -356,21 +356,6 @@
   </si>
   <si>
     <t>User4</t>
-  </si>
-  <si>
-    <t>FA</t>
-  </si>
-  <si>
-    <t>valueA0</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* </t>
-  </si>
-  <si>
-    <t>autosteerData2</t>
   </si>
 </sst>
 </file>
@@ -643,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -785,34 +770,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1121,7 +1100,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1129,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD66"/>
+  <dimension ref="A1:AD64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1147,15 +1126,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -1276,17 +1255,17 @@
       <c r="E5" s="22">
         <v>8</v>
       </c>
-      <c r="F5" s="57" t="s">
+      <c r="F5" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="58"/>
+      <c r="G5" s="52"/>
       <c r="H5" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="59" t="s">
+      <c r="I5" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="60"/>
+      <c r="J5" s="54"/>
       <c r="K5" s="44" t="s">
         <v>24</v>
       </c>
@@ -1337,15 +1316,15 @@
       <c r="F7" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52" t="s">
+      <c r="G7" s="56"/>
+      <c r="H7" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52" t="s">
+      <c r="I7" s="56"/>
+      <c r="J7" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="52"/>
+      <c r="K7" s="56"/>
       <c r="L7" s="44" t="s">
         <v>34</v>
       </c>
@@ -1404,10 +1383,10 @@
       <c r="J9" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="52" t="s">
+      <c r="K9" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="52"/>
+      <c r="L9" s="56"/>
       <c r="M9" s="44" t="s">
         <v>44</v>
       </c>
@@ -1492,126 +1471,125 @@
       <c r="N12" s="44"/>
       <c r="O12" s="44"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="B13" s="50" t="s">
+    <row r="13" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="35"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="39"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="50" t="s">
-        <v>110</v>
-      </c>
-      <c r="D13" s="50">
-        <v>250</v>
-      </c>
-      <c r="E13" s="22">
+      <c r="C14" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="43">
+        <f>HEX2DEC(C14)</f>
+        <v>239</v>
+      </c>
+      <c r="E14" s="22">
         <v>8</v>
       </c>
-      <c r="F13" s="51" t="s">
-        <v>111</v>
-      </c>
-      <c r="G13" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="H13" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="I13" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="J13" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="K13" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="L13" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="M13" s="51" t="s">
-        <v>113</v>
-      </c>
-      <c r="N13" s="51" t="s">
+      <c r="F14" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="K14" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="N14" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="O13" s="51"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51"/>
-      <c r="O14" s="51"/>
-    </row>
-    <row r="15" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="35"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="38"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="39"/>
-      <c r="R15" s="39"/>
+      <c r="O14" s="44"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="44"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="43" t="s">
-        <v>19</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B16" s="43"/>
       <c r="C16" s="43" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D16" s="43">
         <f>HEX2DEC(C16)</f>
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E16" s="22">
         <v>8</v>
       </c>
       <c r="F16" s="44" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G16" s="44" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="H16" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" s="32" t="s">
-        <v>55</v>
+        <v>60</v>
+      </c>
+      <c r="I16" s="44" t="s">
+        <v>47</v>
       </c>
       <c r="J16" s="44" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K16" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="L16" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="M16" s="32" t="s">
-        <v>26</v>
+        <v>107</v>
+      </c>
+      <c r="L16" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="M16" s="44" t="s">
+        <v>109</v>
       </c>
       <c r="N16" s="44" t="s">
         <v>27</v>
@@ -1635,47 +1613,94 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="34" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="B18" s="43"/>
       <c r="C18" s="43" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D18" s="43">
-        <f>HEX2DEC(C18)</f>
-        <v>238</v>
+        <f t="shared" ref="D18" si="0">HEX2DEC(C18)</f>
+        <v>237</v>
       </c>
       <c r="E18" s="22">
+        <v>20</v>
+      </c>
+      <c r="F18" s="44">
+        <v>1</v>
+      </c>
+      <c r="G18" s="44">
+        <v>2</v>
+      </c>
+      <c r="H18" s="44">
+        <v>3</v>
+      </c>
+      <c r="I18" s="44">
+        <v>4</v>
+      </c>
+      <c r="J18" s="44">
+        <v>5</v>
+      </c>
+      <c r="K18" s="44">
+        <v>6</v>
+      </c>
+      <c r="L18" s="44">
+        <v>7</v>
+      </c>
+      <c r="M18" s="44">
         <v>8</v>
       </c>
-      <c r="F18" s="44" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" s="44" t="s">
-        <v>59</v>
-      </c>
-      <c r="H18" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="I18" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="J18" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="K18" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="L18" s="44" t="s">
-        <v>108</v>
-      </c>
-      <c r="M18" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="N18" s="44" t="s">
+      <c r="N18" s="44">
+        <v>9</v>
+      </c>
+      <c r="O18" s="44">
+        <v>10</v>
+      </c>
+      <c r="P18" s="2">
+        <v>11</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>12</v>
+      </c>
+      <c r="R18" s="2">
+        <v>13</v>
+      </c>
+      <c r="S18" s="3">
+        <v>14</v>
+      </c>
+      <c r="T18" s="3">
+        <v>15</v>
+      </c>
+      <c r="U18" s="3">
+        <v>16</v>
+      </c>
+      <c r="V18" s="3">
+        <v>17</v>
+      </c>
+      <c r="W18" s="3">
+        <v>18</v>
+      </c>
+      <c r="X18" s="3">
+        <v>19</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>20</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>21</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>22</v>
+      </c>
+      <c r="AB18" s="3">
+        <v>23</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>24</v>
+      </c>
+      <c r="AD18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="O18" s="44"/>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B19" s="43"/>
@@ -1693,95 +1718,19 @@
       <c r="O19" s="44"/>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A20" s="34" t="s">
-        <v>103</v>
-      </c>
       <c r="B20" s="43"/>
-      <c r="C20" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="43">
-        <f t="shared" ref="D20" si="0">HEX2DEC(C20)</f>
-        <v>237</v>
-      </c>
-      <c r="E20" s="22">
-        <v>20</v>
-      </c>
-      <c r="F20" s="44">
-        <v>1</v>
-      </c>
-      <c r="G20" s="44">
-        <v>2</v>
-      </c>
-      <c r="H20" s="44">
-        <v>3</v>
-      </c>
-      <c r="I20" s="44">
-        <v>4</v>
-      </c>
-      <c r="J20" s="44">
-        <v>5</v>
-      </c>
-      <c r="K20" s="44">
-        <v>6</v>
-      </c>
-      <c r="L20" s="44">
-        <v>7</v>
-      </c>
-      <c r="M20" s="44">
-        <v>8</v>
-      </c>
-      <c r="N20" s="44">
-        <v>9</v>
-      </c>
-      <c r="O20" s="44">
-        <v>10</v>
-      </c>
-      <c r="P20" s="2">
-        <v>11</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>12</v>
-      </c>
-      <c r="R20" s="2">
-        <v>13</v>
-      </c>
-      <c r="S20" s="3">
-        <v>14</v>
-      </c>
-      <c r="T20" s="3">
-        <v>15</v>
-      </c>
-      <c r="U20" s="3">
-        <v>16</v>
-      </c>
-      <c r="V20" s="3">
-        <v>17</v>
-      </c>
-      <c r="W20" s="3">
-        <v>18</v>
-      </c>
-      <c r="X20" s="3">
-        <v>19</v>
-      </c>
-      <c r="Y20" s="3">
-        <v>20</v>
-      </c>
-      <c r="Z20" s="3">
-        <v>21</v>
-      </c>
-      <c r="AA20" s="3">
-        <v>22</v>
-      </c>
-      <c r="AB20" s="3">
-        <v>23</v>
-      </c>
-      <c r="AC20" s="3">
-        <v>24</v>
-      </c>
-      <c r="AD20" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="44"/>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B21" s="43"/>
@@ -1799,19 +1748,46 @@
       <c r="O21" s="44"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="44"/>
-      <c r="O22" s="44"/>
+      <c r="A22" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="43">
+        <v>234</v>
+      </c>
+      <c r="F22" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="I22" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="J22" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="K22" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="L22" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="M22" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="N22" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="O22" s="3"/>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B23" s="43"/>
@@ -1829,46 +1805,19 @@
       <c r="O23" s="44"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A24" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="43">
-        <v>234</v>
-      </c>
-      <c r="F24" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="G24" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="I24" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="J24" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="K24" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="L24" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="M24" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="N24" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="O24" s="3"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B25" s="43"/>
@@ -1885,137 +1834,162 @@
       <c r="N25" s="44"/>
       <c r="O25" s="44"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="44"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="44"/>
-      <c r="M26" s="44"/>
-      <c r="N26" s="44"/>
-      <c r="O26" s="44"/>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="44"/>
-      <c r="O27" s="44"/>
-    </row>
-    <row r="28" spans="1:30" s="40" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="35"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="38"/>
-      <c r="O28" s="38"/>
-      <c r="P28" s="39"/>
-      <c r="Q28" s="39"/>
-      <c r="R28" s="39"/>
-    </row>
-    <row r="29" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="45" t="s">
+    <row r="26" spans="1:30" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="35"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="39"/>
+      <c r="Q26" s="39"/>
+      <c r="R26" s="39"/>
+    </row>
+    <row r="27" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="46" t="s">
+      <c r="B27" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="46" t="s">
+      <c r="C27" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="46">
+      <c r="D27" s="46">
         <v>214</v>
       </c>
-      <c r="E29" s="22" t="s">
+      <c r="E27" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="47"/>
-      <c r="O29" s="47"/>
-      <c r="P29" s="48"/>
-      <c r="Q29" s="48"/>
-      <c r="R29" s="48"/>
-    </row>
-    <row r="30" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="45"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
-      <c r="N30" s="47"/>
-      <c r="O30" s="47"/>
-      <c r="P30" s="48"/>
-      <c r="Q30" s="48"/>
-      <c r="R30" s="48"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="47"/>
+      <c r="M27" s="47"/>
+      <c r="N27" s="47"/>
+      <c r="O27" s="47"/>
+      <c r="P27" s="48"/>
+      <c r="Q27" s="48"/>
+      <c r="R27" s="48"/>
+    </row>
+    <row r="28" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="45"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="47"/>
+      <c r="O28" s="47"/>
+      <c r="P28" s="48"/>
+      <c r="Q28" s="48"/>
+      <c r="R28" s="48"/>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A29" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="43">
+        <v>212</v>
+      </c>
+      <c r="E29" s="22">
+        <v>2</v>
+      </c>
+      <c r="F29" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="H29" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="44"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="44"/>
+      <c r="O29" s="44"/>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B30" s="43"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="44"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="44"/>
+      <c r="O30" s="44"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="34" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B31" s="43" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C31" s="43" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D31" s="43">
-        <v>212</v>
-      </c>
-      <c r="E31" s="22">
-        <v>2</v>
-      </c>
-      <c r="F31" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="H31" s="44" t="s">
+        <f>HEX2DEC(C31)</f>
+        <v>211</v>
+      </c>
+      <c r="E31" s="46">
+        <v>8</v>
+      </c>
+      <c r="F31" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="I31" s="58"/>
+      <c r="J31" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="K31" s="56"/>
+      <c r="L31" s="44">
+        <v>0</v>
+      </c>
+      <c r="M31" s="44">
+        <v>0</v>
+      </c>
+      <c r="N31" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="I31" s="44"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="44"/>
-      <c r="N31" s="44"/>
       <c r="O31" s="44"/>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.2">
@@ -2035,42 +2009,32 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="34" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B33" s="43" t="s">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="C33" s="43" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D33" s="43">
         <f>HEX2DEC(C33)</f>
-        <v>211</v>
-      </c>
-      <c r="E33" s="46">
-        <v>8</v>
-      </c>
-      <c r="F33" s="53" t="s">
-        <v>83</v>
-      </c>
-      <c r="G33" s="54"/>
-      <c r="H33" s="54" t="s">
-        <v>84</v>
-      </c>
-      <c r="I33" s="54"/>
-      <c r="J33" s="52" t="s">
-        <v>99</v>
-      </c>
-      <c r="K33" s="52"/>
-      <c r="L33" s="44">
-        <v>0</v>
-      </c>
-      <c r="M33" s="44">
-        <v>0</v>
-      </c>
-      <c r="N33" s="44" t="s">
-        <v>27</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="44"/>
+      <c r="M33" s="44"/>
+      <c r="N33" s="44"/>
       <c r="O33" s="44"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
@@ -2089,32 +2053,22 @@
       <c r="O34" s="44"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="34" t="s">
-        <v>85</v>
-      </c>
       <c r="B35" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="43" t="s">
-        <v>86</v>
-      </c>
+      <c r="C35" s="43"/>
       <c r="D35" s="43">
         <f>HEX2DEC(C35)</f>
-        <v>210</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="F35" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="44"/>
-      <c r="L35" s="44"/>
-      <c r="M35" s="44"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="56"/>
+      <c r="L35" s="56"/>
+      <c r="M35" s="56"/>
       <c r="N35" s="44"/>
       <c r="O35" s="44"/>
     </row>
@@ -2137,19 +2091,18 @@
       <c r="B37" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43">
-        <f>HEX2DEC(C37)</f>
-        <v>0</v>
-      </c>
-      <c r="F37" s="52"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="52"/>
-      <c r="J37" s="52"/>
-      <c r="K37" s="52"/>
-      <c r="L37" s="52"/>
-      <c r="M37" s="52"/>
+      <c r="C37" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" s="43"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="56"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="56"/>
+      <c r="J37" s="56"/>
+      <c r="K37" s="56"/>
+      <c r="L37" s="56"/>
+      <c r="M37" s="56"/>
       <c r="N37" s="44"/>
       <c r="O37" s="44"/>
     </row>
@@ -2169,21 +2122,28 @@
       <c r="O38" s="44"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" s="34" t="s">
+        <v>102</v>
+      </c>
       <c r="B39" s="43" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="C39" s="43" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="D39" s="43"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="52"/>
-      <c r="I39" s="52"/>
-      <c r="J39" s="52"/>
-      <c r="K39" s="52"/>
-      <c r="L39" s="52"/>
-      <c r="M39" s="52"/>
+      <c r="F39" s="44">
+        <v>1</v>
+      </c>
+      <c r="G39" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="H39" s="44"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="44"/>
+      <c r="L39" s="44"/>
+      <c r="M39" s="44"/>
       <c r="N39" s="44"/>
       <c r="O39" s="44"/>
     </row>
@@ -2203,22 +2163,11 @@
       <c r="O40" s="44"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="B41" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="C41" s="43" t="s">
-        <v>101</v>
-      </c>
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
       <c r="D41" s="43"/>
-      <c r="F41" s="44">
-        <v>1</v>
-      </c>
-      <c r="G41" s="44" t="s">
-        <v>27</v>
-      </c>
+      <c r="F41" s="44"/>
+      <c r="G41" s="44"/>
       <c r="H41" s="44"/>
       <c r="I41" s="44"/>
       <c r="J41" s="44"/>
@@ -2227,21 +2176,6 @@
       <c r="M41" s="44"/>
       <c r="N41" s="44"/>
       <c r="O41" s="44"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B42" s="43"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="43"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44"/>
-      <c r="K42" s="44"/>
-      <c r="L42" s="44"/>
-      <c r="M42" s="44"/>
-      <c r="N42" s="44"/>
-      <c r="O42" s="44"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B43" s="43"/>
@@ -2288,6 +2222,21 @@
       <c r="N47" s="44"/>
       <c r="O47" s="44"/>
     </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B48" s="43"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="44"/>
+      <c r="J48" s="44"/>
+      <c r="K48" s="44"/>
+      <c r="L48" s="44"/>
+      <c r="M48" s="44"/>
+      <c r="N48" s="44"/>
+      <c r="O48" s="44"/>
+    </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B49" s="43"/>
       <c r="C49" s="43"/>
@@ -2333,21 +2282,6 @@
       <c r="N51" s="44"/>
       <c r="O51" s="44"/>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B52" s="43"/>
-      <c r="C52" s="43"/>
-      <c r="D52" s="43"/>
-      <c r="F52" s="44"/>
-      <c r="G52" s="44"/>
-      <c r="H52" s="44"/>
-      <c r="I52" s="44"/>
-      <c r="J52" s="44"/>
-      <c r="K52" s="44"/>
-      <c r="L52" s="44"/>
-      <c r="M52" s="44"/>
-      <c r="N52" s="44"/>
-      <c r="O52" s="44"/>
-    </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B53" s="43"/>
       <c r="C53" s="43"/>
@@ -2378,6 +2312,21 @@
       <c r="N55" s="44"/>
       <c r="O55" s="44"/>
     </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B56" s="43"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="44"/>
+      <c r="H56" s="44"/>
+      <c r="I56" s="44"/>
+      <c r="J56" s="44"/>
+      <c r="K56" s="44"/>
+      <c r="L56" s="44"/>
+      <c r="M56" s="44"/>
+      <c r="N56" s="44"/>
+      <c r="O56" s="44"/>
+    </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B57" s="43"/>
       <c r="C57" s="43"/>
@@ -2498,51 +2447,21 @@
       <c r="N64" s="44"/>
       <c r="O64" s="44"/>
     </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B65" s="43"/>
-      <c r="C65" s="43"/>
-      <c r="D65" s="43"/>
-      <c r="F65" s="44"/>
-      <c r="G65" s="44"/>
-      <c r="H65" s="44"/>
-      <c r="I65" s="44"/>
-      <c r="J65" s="44"/>
-      <c r="K65" s="44"/>
-      <c r="L65" s="44"/>
-      <c r="M65" s="44"/>
-      <c r="N65" s="44"/>
-      <c r="O65" s="44"/>
-    </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B66" s="43"/>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="F66" s="44"/>
-      <c r="G66" s="44"/>
-      <c r="H66" s="44"/>
-      <c r="I66" s="44"/>
-      <c r="J66" s="44"/>
-      <c r="K66" s="44"/>
-      <c r="L66" s="44"/>
-      <c r="M66" s="44"/>
-      <c r="N66" s="44"/>
-      <c r="O66" s="44"/>
-    </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="F35:M35"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="J31:K31"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="J7:K7"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="F37:M37"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="J33:K33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2706,6 +2625,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100168D69F7049F5C4D941A1ED43A3EBF4E" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="6358b93c66be89da512ed1b0037fb663">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ac7999f6-dd20-429f-9c50-d27a0c8de317" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7603896104695ce44c6e748634a25e45" ns2:_="">
     <xsd:import namespace="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
@@ -2869,15 +2797,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2885,6 +2804,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F34BA2AD-7737-4D5E-9A5C-0001377CDA31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2902,14 +2829,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Add Richards steer ino
</commit_message>
<xml_diff>
--- a/Support/PGN 5.1.xlsx
+++ b/Support/PGN 5.1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="115">
   <si>
     <t>Format: 0x80, 0x81, Src, PGN, Length, [Data Bytes], CRC</t>
   </si>
@@ -356,6 +356,21 @@
   </si>
   <si>
     <t>User4</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>valueA0</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* </t>
+  </si>
+  <si>
+    <t>autosteerData2</t>
   </si>
 </sst>
 </file>
@@ -628,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -770,6 +785,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
@@ -780,18 +813,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1100,7 +1121,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1108,10 +1129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD64"/>
+  <dimension ref="A1:AD66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1126,15 +1147,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -1255,17 +1276,17 @@
       <c r="E5" s="22">
         <v>8</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="52"/>
+      <c r="G5" s="58"/>
       <c r="H5" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="53" t="s">
+      <c r="I5" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="54"/>
+      <c r="J5" s="60"/>
       <c r="K5" s="44" t="s">
         <v>24</v>
       </c>
@@ -1316,15 +1337,15 @@
       <c r="F7" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56" t="s">
+      <c r="G7" s="52"/>
+      <c r="H7" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56" t="s">
+      <c r="I7" s="52"/>
+      <c r="J7" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="56"/>
+      <c r="K7" s="52"/>
       <c r="L7" s="44" t="s">
         <v>34</v>
       </c>
@@ -1383,10 +1404,10 @@
       <c r="J9" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="56" t="s">
+      <c r="K9" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="56"/>
+      <c r="L9" s="52"/>
       <c r="M9" s="44" t="s">
         <v>44</v>
       </c>
@@ -1471,125 +1492,126 @@
       <c r="N12" s="44"/>
       <c r="O12" s="44"/>
     </row>
-    <row r="13" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38"/>
-      <c r="O13" s="38"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="39"/>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="50">
+        <v>250</v>
+      </c>
+      <c r="E13" s="22">
+        <v>8</v>
+      </c>
+      <c r="F13" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="G13" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="H13" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="I13" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="J13" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="K13" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="L13" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="M13" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="N13" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13" s="51"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="43">
-        <f>HEX2DEC(C14)</f>
-        <v>239</v>
-      </c>
-      <c r="E14" s="22">
-        <v>8</v>
-      </c>
-      <c r="F14" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="H14" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="J14" s="44" t="s">
-        <v>105</v>
-      </c>
-      <c r="K14" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="L14" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="M14" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="N14" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="O14" s="44"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="44"/>
-      <c r="N15" s="44"/>
-      <c r="O15" s="44"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="51"/>
+    </row>
+    <row r="15" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="35"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="39"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="43"/>
+        <v>51</v>
+      </c>
+      <c r="B16" s="43" t="s">
+        <v>19</v>
+      </c>
       <c r="C16" s="43" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D16" s="43">
         <f>HEX2DEC(C16)</f>
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E16" s="22">
         <v>8</v>
       </c>
       <c r="F16" s="44" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G16" s="44" t="s">
-        <v>59</v>
+        <v>104</v>
       </c>
       <c r="H16" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="I16" s="44" t="s">
-        <v>47</v>
+        <v>54</v>
+      </c>
+      <c r="I16" s="32" t="s">
+        <v>55</v>
       </c>
       <c r="J16" s="44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K16" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="L16" s="44" t="s">
-        <v>108</v>
-      </c>
-      <c r="M16" s="44" t="s">
-        <v>109</v>
+        <v>24</v>
+      </c>
+      <c r="L16" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="32" t="s">
+        <v>26</v>
       </c>
       <c r="N16" s="44" t="s">
         <v>27</v>
@@ -1613,94 +1635,47 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="34" t="s">
-        <v>103</v>
+        <v>56</v>
       </c>
       <c r="B18" s="43"/>
       <c r="C18" s="43" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D18" s="43">
-        <f t="shared" ref="D18" si="0">HEX2DEC(C18)</f>
-        <v>237</v>
+        <f>HEX2DEC(C18)</f>
+        <v>238</v>
       </c>
       <c r="E18" s="22">
-        <v>20</v>
-      </c>
-      <c r="F18" s="44">
-        <v>1</v>
-      </c>
-      <c r="G18" s="44">
-        <v>2</v>
-      </c>
-      <c r="H18" s="44">
-        <v>3</v>
-      </c>
-      <c r="I18" s="44">
-        <v>4</v>
-      </c>
-      <c r="J18" s="44">
-        <v>5</v>
-      </c>
-      <c r="K18" s="44">
-        <v>6</v>
-      </c>
-      <c r="L18" s="44">
-        <v>7</v>
-      </c>
-      <c r="M18" s="44">
         <v>8</v>
       </c>
-      <c r="N18" s="44">
-        <v>9</v>
-      </c>
-      <c r="O18" s="44">
-        <v>10</v>
-      </c>
-      <c r="P18" s="2">
-        <v>11</v>
-      </c>
-      <c r="Q18" s="2">
-        <v>12</v>
-      </c>
-      <c r="R18" s="2">
-        <v>13</v>
-      </c>
-      <c r="S18" s="3">
-        <v>14</v>
-      </c>
-      <c r="T18" s="3">
-        <v>15</v>
-      </c>
-      <c r="U18" s="3">
-        <v>16</v>
-      </c>
-      <c r="V18" s="3">
-        <v>17</v>
-      </c>
-      <c r="W18" s="3">
-        <v>18</v>
-      </c>
-      <c r="X18" s="3">
-        <v>19</v>
-      </c>
-      <c r="Y18" s="3">
-        <v>20</v>
-      </c>
-      <c r="Z18" s="3">
-        <v>21</v>
-      </c>
-      <c r="AA18" s="3">
-        <v>22</v>
-      </c>
-      <c r="AB18" s="3">
-        <v>23</v>
-      </c>
-      <c r="AC18" s="3">
-        <v>24</v>
-      </c>
-      <c r="AD18" s="3" t="s">
+      <c r="F18" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="K18" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="L18" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="M18" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="N18" s="44" t="s">
         <v>27</v>
       </c>
+      <c r="O18" s="44"/>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B19" s="43"/>
@@ -1718,19 +1693,95 @@
       <c r="O19" s="44"/>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A20" s="34" t="s">
+        <v>103</v>
+      </c>
       <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="44"/>
-      <c r="N20" s="44"/>
-      <c r="O20" s="44"/>
+      <c r="C20" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="43">
+        <f t="shared" ref="D20" si="0">HEX2DEC(C20)</f>
+        <v>237</v>
+      </c>
+      <c r="E20" s="22">
+        <v>20</v>
+      </c>
+      <c r="F20" s="44">
+        <v>1</v>
+      </c>
+      <c r="G20" s="44">
+        <v>2</v>
+      </c>
+      <c r="H20" s="44">
+        <v>3</v>
+      </c>
+      <c r="I20" s="44">
+        <v>4</v>
+      </c>
+      <c r="J20" s="44">
+        <v>5</v>
+      </c>
+      <c r="K20" s="44">
+        <v>6</v>
+      </c>
+      <c r="L20" s="44">
+        <v>7</v>
+      </c>
+      <c r="M20" s="44">
+        <v>8</v>
+      </c>
+      <c r="N20" s="44">
+        <v>9</v>
+      </c>
+      <c r="O20" s="44">
+        <v>10</v>
+      </c>
+      <c r="P20" s="2">
+        <v>11</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>12</v>
+      </c>
+      <c r="R20" s="2">
+        <v>13</v>
+      </c>
+      <c r="S20" s="3">
+        <v>14</v>
+      </c>
+      <c r="T20" s="3">
+        <v>15</v>
+      </c>
+      <c r="U20" s="3">
+        <v>16</v>
+      </c>
+      <c r="V20" s="3">
+        <v>17</v>
+      </c>
+      <c r="W20" s="3">
+        <v>18</v>
+      </c>
+      <c r="X20" s="3">
+        <v>19</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>20</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>21</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>22</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>23</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>24</v>
+      </c>
+      <c r="AD20" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B21" s="43"/>
@@ -1748,46 +1799,19 @@
       <c r="O21" s="44"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A22" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="43">
-        <v>234</v>
-      </c>
-      <c r="F22" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="G22" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="H22" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="I22" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="K22" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="L22" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="M22" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="N22" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="O22" s="3"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B23" s="43"/>
@@ -1805,19 +1829,46 @@
       <c r="O23" s="44"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="44"/>
-      <c r="N24" s="44"/>
-      <c r="O24" s="44"/>
+      <c r="A24" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="43">
+        <v>234</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="I24" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="J24" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="K24" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="L24" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="M24" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="N24" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="O24" s="3"/>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B25" s="43"/>
@@ -1834,162 +1885,137 @@
       <c r="N25" s="44"/>
       <c r="O25" s="44"/>
     </row>
-    <row r="26" spans="1:30" s="40" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="35"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
-      <c r="O26" s="38"/>
-      <c r="P26" s="39"/>
-      <c r="Q26" s="39"/>
-      <c r="R26" s="39"/>
-    </row>
-    <row r="27" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="45" t="s">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
+    </row>
+    <row r="28" spans="1:30" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="35"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="39"/>
+      <c r="Q28" s="39"/>
+      <c r="R28" s="39"/>
+    </row>
+    <row r="29" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="46" t="s">
+      <c r="B29" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="46" t="s">
+      <c r="C29" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="46">
+      <c r="D29" s="46">
         <v>214</v>
       </c>
-      <c r="E27" s="22" t="s">
+      <c r="E29" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="47"/>
-      <c r="K27" s="47"/>
-      <c r="L27" s="47"/>
-      <c r="M27" s="47"/>
-      <c r="N27" s="47"/>
-      <c r="O27" s="47"/>
-      <c r="P27" s="48"/>
-      <c r="Q27" s="48"/>
-      <c r="R27" s="48"/>
-    </row>
-    <row r="28" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="45"/>
-      <c r="B28" s="46"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="47"/>
-      <c r="O28" s="47"/>
-      <c r="P28" s="48"/>
-      <c r="Q28" s="48"/>
-      <c r="R28" s="48"/>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A29" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B29" s="43" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="43">
-        <v>212</v>
-      </c>
-      <c r="E29" s="22">
-        <v>2</v>
-      </c>
-      <c r="F29" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="G29" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="H29" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="44"/>
-      <c r="N29" s="44"/>
-      <c r="O29" s="44"/>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="44"/>
-      <c r="L30" s="44"/>
-      <c r="M30" s="44"/>
-      <c r="N30" s="44"/>
-      <c r="O30" s="44"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="47"/>
+      <c r="P29" s="48"/>
+      <c r="Q29" s="48"/>
+      <c r="R29" s="48"/>
+    </row>
+    <row r="30" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="45"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="47"/>
+      <c r="O30" s="47"/>
+      <c r="P30" s="48"/>
+      <c r="Q30" s="48"/>
+      <c r="R30" s="48"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="34" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B31" s="43" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C31" s="43" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D31" s="43">
-        <f>HEX2DEC(C31)</f>
-        <v>211</v>
-      </c>
-      <c r="E31" s="46">
-        <v>8</v>
-      </c>
-      <c r="F31" s="57" t="s">
-        <v>83</v>
-      </c>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58" t="s">
-        <v>84</v>
-      </c>
-      <c r="I31" s="58"/>
-      <c r="J31" s="56" t="s">
-        <v>99</v>
-      </c>
-      <c r="K31" s="56"/>
-      <c r="L31" s="44">
-        <v>0</v>
-      </c>
-      <c r="M31" s="44">
-        <v>0</v>
-      </c>
-      <c r="N31" s="44" t="s">
+        <v>212</v>
+      </c>
+      <c r="E31" s="22">
+        <v>2</v>
+      </c>
+      <c r="F31" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="H31" s="44" t="s">
         <v>27</v>
       </c>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="44"/>
+      <c r="L31" s="44"/>
+      <c r="M31" s="44"/>
+      <c r="N31" s="44"/>
       <c r="O31" s="44"/>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.2">
@@ -2009,32 +2035,42 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="34" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B33" s="43" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C33" s="43" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D33" s="43">
         <f>HEX2DEC(C33)</f>
-        <v>210</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="F33" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="44"/>
-      <c r="K33" s="44"/>
-      <c r="L33" s="44"/>
-      <c r="M33" s="44"/>
-      <c r="N33" s="44"/>
+        <v>211</v>
+      </c>
+      <c r="E33" s="46">
+        <v>8</v>
+      </c>
+      <c r="F33" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="G33" s="54"/>
+      <c r="H33" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="I33" s="54"/>
+      <c r="J33" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="K33" s="52"/>
+      <c r="L33" s="44">
+        <v>0</v>
+      </c>
+      <c r="M33" s="44">
+        <v>0</v>
+      </c>
+      <c r="N33" s="44" t="s">
+        <v>27</v>
+      </c>
       <c r="O33" s="44"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
@@ -2053,22 +2089,32 @@
       <c r="O34" s="44"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="34" t="s">
+        <v>85</v>
+      </c>
       <c r="B35" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="43"/>
+      <c r="C35" s="43" t="s">
+        <v>86</v>
+      </c>
       <c r="D35" s="43">
         <f>HEX2DEC(C35)</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="56"/>
-      <c r="K35" s="56"/>
-      <c r="L35" s="56"/>
-      <c r="M35" s="56"/>
+        <v>210</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="44"/>
+      <c r="M35" s="44"/>
       <c r="N35" s="44"/>
       <c r="O35" s="44"/>
     </row>
@@ -2091,18 +2137,19 @@
       <c r="B37" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="D37" s="43"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="56"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="56"/>
-      <c r="M37" s="56"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43">
+        <f>HEX2DEC(C37)</f>
+        <v>0</v>
+      </c>
+      <c r="F37" s="52"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="52"/>
+      <c r="L37" s="52"/>
+      <c r="M37" s="52"/>
       <c r="N37" s="44"/>
       <c r="O37" s="44"/>
     </row>
@@ -2122,28 +2169,21 @@
       <c r="O38" s="44"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="34" t="s">
-        <v>102</v>
-      </c>
       <c r="B39" s="43" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="C39" s="43" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D39" s="43"/>
-      <c r="F39" s="44">
-        <v>1</v>
-      </c>
-      <c r="G39" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="H39" s="44"/>
-      <c r="I39" s="44"/>
-      <c r="J39" s="44"/>
-      <c r="K39" s="44"/>
-      <c r="L39" s="44"/>
-      <c r="M39" s="44"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="52"/>
+      <c r="I39" s="52"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="52"/>
+      <c r="L39" s="52"/>
+      <c r="M39" s="52"/>
       <c r="N39" s="44"/>
       <c r="O39" s="44"/>
     </row>
@@ -2163,11 +2203,22 @@
       <c r="O40" s="44"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
+      <c r="A41" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="43" t="s">
+        <v>101</v>
+      </c>
       <c r="D41" s="43"/>
-      <c r="F41" s="44"/>
-      <c r="G41" s="44"/>
+      <c r="F41" s="44">
+        <v>1</v>
+      </c>
+      <c r="G41" s="44" t="s">
+        <v>27</v>
+      </c>
       <c r="H41" s="44"/>
       <c r="I41" s="44"/>
       <c r="J41" s="44"/>
@@ -2176,6 +2227,21 @@
       <c r="M41" s="44"/>
       <c r="N41" s="44"/>
       <c r="O41" s="44"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B42" s="43"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44"/>
+      <c r="K42" s="44"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="44"/>
+      <c r="N42" s="44"/>
+      <c r="O42" s="44"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B43" s="43"/>
@@ -2222,21 +2288,6 @@
       <c r="N47" s="44"/>
       <c r="O47" s="44"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="F48" s="44"/>
-      <c r="G48" s="44"/>
-      <c r="H48" s="44"/>
-      <c r="I48" s="44"/>
-      <c r="J48" s="44"/>
-      <c r="K48" s="44"/>
-      <c r="L48" s="44"/>
-      <c r="M48" s="44"/>
-      <c r="N48" s="44"/>
-      <c r="O48" s="44"/>
-    </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B49" s="43"/>
       <c r="C49" s="43"/>
@@ -2282,6 +2333,21 @@
       <c r="N51" s="44"/>
       <c r="O51" s="44"/>
     </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B52" s="43"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="43"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
+      <c r="H52" s="44"/>
+      <c r="I52" s="44"/>
+      <c r="J52" s="44"/>
+      <c r="K52" s="44"/>
+      <c r="L52" s="44"/>
+      <c r="M52" s="44"/>
+      <c r="N52" s="44"/>
+      <c r="O52" s="44"/>
+    </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B53" s="43"/>
       <c r="C53" s="43"/>
@@ -2312,21 +2378,6 @@
       <c r="N55" s="44"/>
       <c r="O55" s="44"/>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B56" s="43"/>
-      <c r="C56" s="43"/>
-      <c r="D56" s="43"/>
-      <c r="F56" s="44"/>
-      <c r="G56" s="44"/>
-      <c r="H56" s="44"/>
-      <c r="I56" s="44"/>
-      <c r="J56" s="44"/>
-      <c r="K56" s="44"/>
-      <c r="L56" s="44"/>
-      <c r="M56" s="44"/>
-      <c r="N56" s="44"/>
-      <c r="O56" s="44"/>
-    </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B57" s="43"/>
       <c r="C57" s="43"/>
@@ -2447,21 +2498,51 @@
       <c r="N64" s="44"/>
       <c r="O64" s="44"/>
     </row>
+    <row r="65" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B65" s="43"/>
+      <c r="C65" s="43"/>
+      <c r="D65" s="43"/>
+      <c r="F65" s="44"/>
+      <c r="G65" s="44"/>
+      <c r="H65" s="44"/>
+      <c r="I65" s="44"/>
+      <c r="J65" s="44"/>
+      <c r="K65" s="44"/>
+      <c r="L65" s="44"/>
+      <c r="M65" s="44"/>
+      <c r="N65" s="44"/>
+      <c r="O65" s="44"/>
+    </row>
+    <row r="66" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B66" s="43"/>
+      <c r="C66" s="43"/>
+      <c r="D66" s="43"/>
+      <c r="F66" s="44"/>
+      <c r="G66" s="44"/>
+      <c r="H66" s="44"/>
+      <c r="I66" s="44"/>
+      <c r="J66" s="44"/>
+      <c r="K66" s="44"/>
+      <c r="L66" s="44"/>
+      <c r="M66" s="44"/>
+      <c r="N66" s="44"/>
+      <c r="O66" s="44"/>
+    </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="F35:M35"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="J31:K31"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="J7:K7"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="F37:M37"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="J33:K33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2625,15 +2706,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100168D69F7049F5C4D941A1ED43A3EBF4E" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="6358b93c66be89da512ed1b0037fb663">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ac7999f6-dd20-429f-9c50-d27a0c8de317" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7603896104695ce44c6e748634a25e45" ns2:_="">
     <xsd:import namespace="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
@@ -2797,6 +2869,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2804,14 +2885,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F34BA2AD-7737-4D5E-9A5C-0001377CDA31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2829,6 +2902,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
   <ds:schemaRefs>

</xml_diff>